<commit_message>
atualiza ficha de projeto e bases de dados que serão utilizadas
</commit_message>
<xml_diff>
--- a/Ficha projeto.xlsx
+++ b/Ficha projeto.xlsx
@@ -37,63 +37,7 @@
     <t>Banco de dados</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Postagens em 4 fóruns diferentes do curso de Citologia, da UPE, onde para cada fórum o primeiro post é contém uma temática sugerida pelo professor, e os posts seguintes são as respostas dos alunos. Podendo os mesmos responderem ao post temático ou ao post de outros alunos. O nome dos 4 fóruns, e a quantidade de postagens respectivas para cada um (incluindo postagens do professor respondendo a posts dos alunos, somando </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t xml:space="preserve">385 posts </t>
-    </r>
-    <r>
-      <t xml:space="preserve">no total dos 4 fóruns), são: “1º FÓRUM TEMÁTICO: QUAIS AS TRANSFORMAÇÕES OCORRIDAS COM O USO DO MICROSCÓPIO NA SOCIEDADE?”, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t>511</t>
-    </r>
-    <r>
-      <t xml:space="preserve">; "2º FÓRUM TEMÁTICO: A PROBLEMÁTICA É SIMPLES: QUANDO COMEÇA E QUANDO TERMINA A VIDA DE UM SER VIVO" , </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t>400</t>
-    </r>
-    <r>
-      <t xml:space="preserve">; “3º FÓRUM TEMÁTICO: QUAIS OS PONTOS POSITIVOS E NEGATIVOS DA CLONAGEM?”, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t>314</t>
-    </r>
-    <r>
-      <t xml:space="preserve">; "4º FÓRUM TEMÁTICO: COMO SERIA NOSSA SOCIEDADE APÓS A CONCRETIZAÇÃO DA POSSIBILIDADE DE MANIPULAÇÃO DOS GENES BASEADO NO FILME GATTACA - EXPERIÊNCIA GENÉTICA (1997)?", </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t>275</t>
-    </r>
-    <r>
-      <t xml:space="preserve">. Totalizando </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t>1500</t>
-    </r>
-    <r>
-      <t xml:space="preserve"> posts.</t>
-    </r>
+    <t>Postagens em 4 fóruns diferentes do curso de Psicologia do Desenvolvimento, da UPE, onde para cada fórum o primeiro post é contém uma temática sugerida pelo professor, e os posts seguintes são as respostas dos alunos. Podendo os mesmos responderem ao post temático ou ao post de outros alunos. O nome dos 4 fóruns, e a quantidade de postagens respectivas para cada um (considerando somente os posts dos alunos), são: “1º FÓRUM TEMÁTICO: “Pau que nasce torto morre torto””, 443; "2º FÓRUM TEMÁTICO: "O Tamanho é de Uma Criança, Mas o Comportamento é de Um Adulto"" , 303; “3º FÓRUM TEMÁTICO:: “NÃO VOU ME ADAPTAR””, 268; "4º FÓRUM TEMÁTICO: A escola que afirma não ter bullying ou não sabe o que é, ou está negando a sua existência.", 264. Totalizando 1278 posts de alunos. E um total de 374 posts de feedback do professor, misturado entre os 4 fóruns.</t>
   </si>
   <si>
     <t>Entregas</t>
@@ -262,7 +206,7 @@
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -275,7 +219,7 @@
     <xf borderId="4" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -542,7 +486,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" ht="267.0" customHeight="1">
+    <row r="6" ht="222.75" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -581,22 +525,22 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="11" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>